<commit_message>
ThematicArea and type added
</commit_message>
<xml_diff>
--- a/source-data/dataTrento/dataTrento.xlsx
+++ b/source-data/dataTrento/dataTrento.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="834">
   <si>
     <t>PSDURI</t>
   </si>
@@ -2972,6 +2972,9 @@
   </si>
   <si>
     <t>R90 - Creative, arts and entertainment activities</t>
+  </si>
+  <si>
+    <t>08.2 - Cultural services</t>
   </si>
 </sst>
 </file>
@@ -11882,8 +11885,8 @@
   </sheetPr>
   <dimension ref="A1:Z1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12017,7 +12020,7 @@
         <v>35</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>804</v>
+        <v>833</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Last fixes to the spreadsheet
</commit_message>
<xml_diff>
--- a/source-data/dataTrento/dataTrento.xlsx
+++ b/source-data/dataTrento/dataTrento.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\servaism\Documents\1-Clients\CPSV-AP\Trento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\servaism\git\Trento_conversionToRDF\source-data\dataTrento\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6765" firstSheet="4" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6765" firstSheet="6" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Public Service" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="340">
   <si>
     <t>Name</t>
   </si>
@@ -1099,6 +1099,30 @@
   </si>
   <si>
     <t>Per la federazione trentina delle associazioni proloco e consorzi: domanda di contributo con relazione illustrativa dell’attività e piano finanziario</t>
+  </si>
+  <si>
+    <t>Provincia Autonoma di Trento - Servizio attività culturali</t>
+  </si>
+  <si>
+    <t>via Romagnosi 5 - 38122 Trento</t>
+  </si>
+  <si>
+    <t>Provincia Autonoma di Trento - Servizio agricoltura</t>
+  </si>
+  <si>
+    <t>via Trener 3 - 38122 Trento</t>
+  </si>
+  <si>
+    <t>Provincia Autonoma di Trento - Agenzia provinciale per la protezione dell'ambiente</t>
+  </si>
+  <si>
+    <t>piazza Vittoria 5 - 38122 Trento</t>
+  </si>
+  <si>
+    <t>Provincia Autonoma di Trento - Servizio turismo e sport</t>
+  </si>
+  <si>
+    <t>via Romagnosi 9 - 38122 Trento</t>
   </si>
 </sst>
 </file>
@@ -1236,7 +1260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1322,6 +1346,24 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1717,8 +1759,8 @@
   <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15"/>
@@ -2843,7 +2885,7 @@
   </sheetPr>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
@@ -3084,11 +3126,11 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -3096,120 +3138,96 @@
     <col min="1" max="1" width="26.85546875" customWidth="1"/>
     <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="22.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="27.75" customHeight="1">
+      <c r="A1" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+    <row r="2" spans="1:9" ht="42.75">
+      <c r="A2" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>332</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" s="43"/>
+      <c r="F2" s="44" t="s">
+        <v>333</v>
+      </c>
+      <c r="I2" s="44"/>
+    </row>
+    <row r="3" spans="1:9" ht="42.75">
+      <c r="A3" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>334</v>
+      </c>
+      <c r="C3" s="43"/>
+      <c r="D3" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="E3" s="43"/>
+      <c r="F3" s="45" t="s">
+        <v>335</v>
+      </c>
+      <c r="I3" s="44"/>
+    </row>
+    <row r="4" spans="1:9" ht="45">
+      <c r="A4" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>336</v>
+      </c>
+      <c r="C4" s="43"/>
+      <c r="D4" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" s="43"/>
+      <c r="F4" s="45" t="s">
+        <v>337</v>
+      </c>
+      <c r="I4" s="45"/>
+    </row>
+    <row r="5" spans="1:9" ht="42.75">
+      <c r="A5" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>338</v>
+      </c>
+      <c r="C5" s="43"/>
+      <c r="D5" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" s="43"/>
+      <c r="F5" s="45" t="s">
+        <v>339</v>
+      </c>
+      <c r="I5" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4661,75 +4679,14 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PwC_JobCode xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">F049</PwC_JobCode>
-    <PwC_JobSearch xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">F049 - ABCIII SC270</PwC_JobSearch>
-    <PwC_FiscalYear xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">FY17</PwC_FiscalYear>
-    <PwC_Language xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">EN</PwC_Language>
-    <PwC_ExpirationDate xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">2023-07-10T22:00:00+00:00</PwC_ExpirationDate>
-    <PwC_ClientCode xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">86155139</PwC_ClientCode>
-    <RelatedItems xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PwC_ClientSearch xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">86155139 - DG INFORMATICS (DIGIT)</PwC_ClientSearch>
-    <_dlc_DocId xmlns="73fde05d-ef26-44d0-b13b-b564e323f6a1">SK445ZKHUCMR-447-133</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="73fde05d-ef26-44d0-b13b-b564e323f6a1">
-      <Url>https://be-docbox.be.ema.pwcinternal.com/sites/10014628/86155139F049/_layouts/15/DocIdRedir.aspx?ID=SK445ZKHUCMR-447-133</Url>
-      <Description>SK445ZKHUCMR-447-133</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="PwC Job Document" ma:contentTypeID="0x0101008E49C3D400044AB3A2F1DD14073E74F6001D06D12572244BE3A11AAEE3ED60F576000AAB1FD6C2134AF1A3EA6F52344189D8003DA7CBE2F9F6014D91228B237B0D6438" ma:contentTypeVersion="2" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="3d6a3c6679c05d12a3160ad00a1d5007">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="73fde05d-ef26-44d0-b13b-b564e323f6a1" xmlns:ns3="885fffe5-095f-4e72-b33a-2965af2fc427" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e9ac53f853e0ef9b3d9397434b7eb735" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4940,42 +4897,85 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PwC_JobCode xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">F049</PwC_JobCode>
+    <PwC_JobSearch xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">F049 - ABCIII SC270</PwC_JobSearch>
+    <PwC_FiscalYear xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">FY17</PwC_FiscalYear>
+    <PwC_Language xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">EN</PwC_Language>
+    <PwC_ExpirationDate xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">2023-07-10T22:00:00+00:00</PwC_ExpirationDate>
+    <PwC_ClientCode xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">86155139</PwC_ClientCode>
+    <RelatedItems xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PwC_ClientSearch xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">86155139 - DG INFORMATICS (DIGIT)</PwC_ClientSearch>
+    <_dlc_DocId xmlns="73fde05d-ef26-44d0-b13b-b564e323f6a1">SK445ZKHUCMR-447-133</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="73fde05d-ef26-44d0-b13b-b564e323f6a1">
+      <Url>https://be-docbox.be.ema.pwcinternal.com/sites/10014628/86155139F049/_layouts/15/DocIdRedir.aspx?ID=SK445ZKHUCMR-447-133</Url>
+      <Description>SK445ZKHUCMR-447-133</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704B0184-4F17-45F2-9AC0-8A30DB782E6F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08E82FCB-F73C-4EEA-86B9-8873465BC0AE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B2323CD-3102-47C1-AE6C-40C0EBF3BFA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="73fde05d-ef26-44d0-b13b-b564e323f6a1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="885fffe5-095f-4e72-b33a-2965af2fc427"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10E94497-4933-4E21-9510-AD09FE48006D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4995,10 +4995,28 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B2323CD-3102-47C1-AE6C-40C0EBF3BFA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="73fde05d-ef26-44d0-b13b-b564e323f6a1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="885fffe5-095f-4e72-b33a-2965af2fc427"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08E82FCB-F73C-4EEA-86B9-8873465BC0AE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704B0184-4F17-45F2-9AC0-8A30DB782E6F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adapted exceljson_Trento.js in light of changes of source data
</commit_message>
<xml_diff>
--- a/source-data/dataTrento/dataTrento.xlsx
+++ b/source-data/dataTrento/dataTrento.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6765" firstSheet="6" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6765" firstSheet="12" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Public Service" sheetId="2" r:id="rId1"/>
@@ -1759,8 +1759,8 @@
   <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D10"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15"/>
@@ -2512,7 +2512,9 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -3128,7 +3130,7 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
@@ -3241,7 +3243,7 @@
   </sheetPr>
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -3415,7 +3417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3697,7 +3699,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -4004,9 +4006,9 @@
   </sheetPr>
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -4327,7 +4329,7 @@
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -4606,7 +4608,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -4679,14 +4681,75 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PwC_JobCode xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">F049</PwC_JobCode>
+    <PwC_JobSearch xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">F049 - ABCIII SC270</PwC_JobSearch>
+    <PwC_FiscalYear xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">FY17</PwC_FiscalYear>
+    <PwC_Language xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">EN</PwC_Language>
+    <PwC_ExpirationDate xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">2023-07-10T22:00:00+00:00</PwC_ExpirationDate>
+    <PwC_ClientCode xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">86155139</PwC_ClientCode>
+    <RelatedItems xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PwC_ClientSearch xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">86155139 - DG INFORMATICS (DIGIT)</PwC_ClientSearch>
+    <_dlc_DocId xmlns="73fde05d-ef26-44d0-b13b-b564e323f6a1">SK445ZKHUCMR-447-133</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="73fde05d-ef26-44d0-b13b-b564e323f6a1">
+      <Url>https://be-docbox.be.ema.pwcinternal.com/sites/10014628/86155139F049/_layouts/15/DocIdRedir.aspx?ID=SK445ZKHUCMR-447-133</Url>
+      <Description>SK445ZKHUCMR-447-133</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="PwC Job Document" ma:contentTypeID="0x0101008E49C3D400044AB3A2F1DD14073E74F6001D06D12572244BE3A11AAEE3ED60F576000AAB1FD6C2134AF1A3EA6F52344189D8003DA7CBE2F9F6014D91228B237B0D6438" ma:contentTypeVersion="2" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="3d6a3c6679c05d12a3160ad00a1d5007">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="73fde05d-ef26-44d0-b13b-b564e323f6a1" xmlns:ns3="885fffe5-095f-4e72-b33a-2965af2fc427" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e9ac53f853e0ef9b3d9397434b7eb735" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4897,85 +4960,42 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PwC_JobCode xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">F049</PwC_JobCode>
-    <PwC_JobSearch xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">F049 - ABCIII SC270</PwC_JobSearch>
-    <PwC_FiscalYear xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">FY17</PwC_FiscalYear>
-    <PwC_Language xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">EN</PwC_Language>
-    <PwC_ExpirationDate xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">2023-07-10T22:00:00+00:00</PwC_ExpirationDate>
-    <PwC_ClientCode xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">86155139</PwC_ClientCode>
-    <RelatedItems xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PwC_ClientSearch xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">86155139 - DG INFORMATICS (DIGIT)</PwC_ClientSearch>
-    <_dlc_DocId xmlns="73fde05d-ef26-44d0-b13b-b564e323f6a1">SK445ZKHUCMR-447-133</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="73fde05d-ef26-44d0-b13b-b564e323f6a1">
-      <Url>https://be-docbox.be.ema.pwcinternal.com/sites/10014628/86155139F049/_layouts/15/DocIdRedir.aspx?ID=SK445ZKHUCMR-447-133</Url>
-      <Description>SK445ZKHUCMR-447-133</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08E82FCB-F73C-4EEA-86B9-8873465BC0AE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704B0184-4F17-45F2-9AC0-8A30DB782E6F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B2323CD-3102-47C1-AE6C-40C0EBF3BFA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="73fde05d-ef26-44d0-b13b-b564e323f6a1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="885fffe5-095f-4e72-b33a-2965af2fc427"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10E94497-4933-4E21-9510-AD09FE48006D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4995,28 +5015,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B2323CD-3102-47C1-AE6C-40C0EBF3BFA9}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08E82FCB-F73C-4EEA-86B9-8873465BC0AE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="73fde05d-ef26-44d0-b13b-b564e323f6a1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="885fffe5-095f-4e72-b33a-2965af2fc427"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704B0184-4F17-45F2-9AC0-8A30DB782E6F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Related & Requires of Class Public Service work
</commit_message>
<xml_diff>
--- a/source-data/dataTrento/dataTrento.xlsx
+++ b/source-data/dataTrento/dataTrento.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6765" firstSheet="12" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6765" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Public Service" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="340">
   <si>
     <t>Name</t>
   </si>
@@ -1758,9 +1758,9 @@
   </sheetPr>
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15"/>
@@ -3130,9 +3130,9 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -3170,7 +3170,9 @@
       <c r="B2" s="44" t="s">
         <v>332</v>
       </c>
-      <c r="C2" s="43"/>
+      <c r="C2" s="44" t="s">
+        <v>332</v>
+      </c>
       <c r="D2" s="44" t="s">
         <v>151</v>
       </c>
@@ -3180,14 +3182,16 @@
       </c>
       <c r="I2" s="44"/>
     </row>
-    <row r="3" spans="1:9" ht="42.75">
+    <row r="3" spans="1:9" ht="45">
       <c r="A3" s="45" t="s">
         <v>102</v>
       </c>
       <c r="B3" s="45" t="s">
         <v>334</v>
       </c>
-      <c r="C3" s="43"/>
+      <c r="C3" s="45" t="s">
+        <v>334</v>
+      </c>
       <c r="D3" s="44" t="s">
         <v>151</v>
       </c>
@@ -3197,14 +3201,16 @@
       </c>
       <c r="I3" s="44"/>
     </row>
-    <row r="4" spans="1:9" ht="45">
+    <row r="4" spans="1:9" ht="75">
       <c r="A4" s="45" t="s">
         <v>103</v>
       </c>
       <c r="B4" s="45" t="s">
         <v>336</v>
       </c>
-      <c r="C4" s="43"/>
+      <c r="C4" s="45" t="s">
+        <v>336</v>
+      </c>
       <c r="D4" s="44" t="s">
         <v>151</v>
       </c>
@@ -3221,7 +3227,9 @@
       <c r="B5" s="44" t="s">
         <v>338</v>
       </c>
-      <c r="C5" s="43"/>
+      <c r="C5" s="44" t="s">
+        <v>338</v>
+      </c>
       <c r="D5" s="44" t="s">
         <v>151</v>
       </c>
@@ -3417,7 +3425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -4681,75 +4689,14 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PwC_JobCode xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">F049</PwC_JobCode>
-    <PwC_JobSearch xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">F049 - ABCIII SC270</PwC_JobSearch>
-    <PwC_FiscalYear xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">FY17</PwC_FiscalYear>
-    <PwC_Language xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">EN</PwC_Language>
-    <PwC_ExpirationDate xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">2023-07-10T22:00:00+00:00</PwC_ExpirationDate>
-    <PwC_ClientCode xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">86155139</PwC_ClientCode>
-    <RelatedItems xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PwC_ClientSearch xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">86155139 - DG INFORMATICS (DIGIT)</PwC_ClientSearch>
-    <_dlc_DocId xmlns="73fde05d-ef26-44d0-b13b-b564e323f6a1">SK445ZKHUCMR-447-133</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="73fde05d-ef26-44d0-b13b-b564e323f6a1">
-      <Url>https://be-docbox.be.ema.pwcinternal.com/sites/10014628/86155139F049/_layouts/15/DocIdRedir.aspx?ID=SK445ZKHUCMR-447-133</Url>
-      <Description>SK445ZKHUCMR-447-133</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="PwC Job Document" ma:contentTypeID="0x0101008E49C3D400044AB3A2F1DD14073E74F6001D06D12572244BE3A11AAEE3ED60F576000AAB1FD6C2134AF1A3EA6F52344189D8003DA7CBE2F9F6014D91228B237B0D6438" ma:contentTypeVersion="2" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="3d6a3c6679c05d12a3160ad00a1d5007">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="73fde05d-ef26-44d0-b13b-b564e323f6a1" xmlns:ns3="885fffe5-095f-4e72-b33a-2965af2fc427" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e9ac53f853e0ef9b3d9397434b7eb735" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4960,42 +4907,85 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PwC_JobCode xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">F049</PwC_JobCode>
+    <PwC_JobSearch xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">F049 - ABCIII SC270</PwC_JobSearch>
+    <PwC_FiscalYear xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">FY17</PwC_FiscalYear>
+    <PwC_Language xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">EN</PwC_Language>
+    <PwC_ExpirationDate xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">2023-07-10T22:00:00+00:00</PwC_ExpirationDate>
+    <PwC_ClientCode xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">86155139</PwC_ClientCode>
+    <RelatedItems xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PwC_ClientSearch xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">86155139 - DG INFORMATICS (DIGIT)</PwC_ClientSearch>
+    <_dlc_DocId xmlns="73fde05d-ef26-44d0-b13b-b564e323f6a1">SK445ZKHUCMR-447-133</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="73fde05d-ef26-44d0-b13b-b564e323f6a1">
+      <Url>https://be-docbox.be.ema.pwcinternal.com/sites/10014628/86155139F049/_layouts/15/DocIdRedir.aspx?ID=SK445ZKHUCMR-447-133</Url>
+      <Description>SK445ZKHUCMR-447-133</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704B0184-4F17-45F2-9AC0-8A30DB782E6F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08E82FCB-F73C-4EEA-86B9-8873465BC0AE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B2323CD-3102-47C1-AE6C-40C0EBF3BFA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="73fde05d-ef26-44d0-b13b-b564e323f6a1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="885fffe5-095f-4e72-b33a-2965af2fc427"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10E94497-4933-4E21-9510-AD09FE48006D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5015,10 +5005,28 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B2323CD-3102-47C1-AE6C-40C0EBF3BFA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="73fde05d-ef26-44d0-b13b-b564e323f6a1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="885fffe5-095f-4e72-b33a-2965af2fc427"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08E82FCB-F73C-4EEA-86B9-8873465BC0AE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704B0184-4F17-45F2-9AC0-8A30DB782E6F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Lot of improvements + some errors were fixed
</commit_message>
<xml_diff>
--- a/source-data/dataTrento/dataTrento.xlsx
+++ b/source-data/dataTrento/dataTrento.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6765" firstSheet="10" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6765"/>
   </bookViews>
   <sheets>
     <sheet name="Public Service" sheetId="2" r:id="rId1"/>
@@ -478,13 +478,7 @@
     <t>p_TN_1665; p_TN_398; p_TN_407; p_TN_402; p_TN_399; p_TN_397; p_TN_396</t>
   </si>
   <si>
-    <t>p_TN_403; p_TN_396; p_TN_407; p_TN_1529;p_TN_402; p_TN_397; p_TN_399</t>
-  </si>
-  <si>
     <t>p_TN_403; p_TN_397; p_TN_1529; p_TN_402; p_TN_396; p_TN_399; p_TN_407</t>
-  </si>
-  <si>
-    <t>p_TN_403; p_ TN_397; p_TN_398; p_TN_1529; p_TN_396; p_TN_399; p_TN_402; p_TN_407</t>
   </si>
   <si>
     <t>p_TN_708; P_TN_704</t>
@@ -1123,6 +1117,12 @@
   </si>
   <si>
     <t>via Romagnosi 9 - 38122 Trento</t>
+  </si>
+  <si>
+    <t>p_TN_403; p_TN_396; p_TN_407; p_TN_1529; p_TN_402; p_TN_397; p_TN_399</t>
+  </si>
+  <si>
+    <t>p_TN_403; p_TN_397; p_TN_398; p_TN_1529; p_TN_396; p_TN_399; p_TN_402; p_TN_407</t>
   </si>
 </sst>
 </file>
@@ -1758,9 +1758,9 @@
   </sheetPr>
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N3" sqref="N3:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15"/>
@@ -1893,7 +1893,7 @@
         <v>105</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H2" s="26" t="s">
         <v>111</v>
@@ -1913,31 +1913,31 @@
       </c>
       <c r="N2" s="24"/>
       <c r="P2" s="23" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="Q2" s="23" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="T2" s="23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="V2" s="19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="W2" s="23" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="X2" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:26" s="2" customFormat="1" ht="69.95" customHeight="1">
@@ -1960,7 +1960,7 @@
         <v>106</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H3" s="26" t="s">
         <v>112</v>
@@ -1979,34 +1979,34 @@
         <v>137</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="P3" s="31" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="Q3" s="23" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="T3" s="23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="V3" s="19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="W3" s="31" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="69.95" customHeight="1">
@@ -2029,7 +2029,7 @@
         <v>107</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H4" s="26" t="s">
         <v>113</v>
@@ -2050,27 +2050,27 @@
       <c r="N4" s="22"/>
       <c r="O4"/>
       <c r="P4" s="31" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="Q4" s="31" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="R4" s="25"/>
       <c r="T4" s="23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="V4" s="19" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="W4" s="25"/>
       <c r="X4" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="69.95" customHeight="1">
@@ -2093,7 +2093,7 @@
         <v>108</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H5" s="27" t="s">
         <v>114</v>
@@ -2114,35 +2114,35 @@
         <v>138</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="O5"/>
       <c r="P5" s="31" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="Q5" s="23" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="T5" s="23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="V5" s="19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="W5" s="23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="X5" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="69.95" customHeight="1">
@@ -2165,7 +2165,7 @@
         <v>105</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H6" s="27" t="s">
         <v>111</v>
@@ -2183,37 +2183,37 @@
         <v>133</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>139</v>
+        <v>338</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="P6" s="31" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="Q6" s="23" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="T6" s="23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="V6" s="19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="W6" s="23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="69.95" customHeight="1">
@@ -2236,7 +2236,7 @@
         <v>105</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H7" s="27" t="s">
         <v>111</v>
@@ -2254,37 +2254,37 @@
         <v>133</v>
       </c>
       <c r="M7" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N7" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="P7" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q7" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="R7" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="P7" s="31" t="s">
-        <v>256</v>
-      </c>
-      <c r="Q7" s="23" t="s">
-        <v>304</v>
-      </c>
-      <c r="R7" s="5" t="s">
-        <v>189</v>
-      </c>
       <c r="T7" s="23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="V7" s="19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="W7" s="23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="69.95" customHeight="1">
@@ -2307,7 +2307,7 @@
         <v>105</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H8" s="27" t="s">
         <v>111</v>
@@ -2325,37 +2325,37 @@
         <v>133</v>
       </c>
       <c r="M8" s="24" t="s">
-        <v>141</v>
+        <v>339</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="P8" s="31" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="Q8" s="23" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="T8" s="23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="V8" s="19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="W8" s="23" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="69.95" customHeight="1">
@@ -2378,7 +2378,7 @@
         <v>109</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H9" s="27" t="s">
         <v>115</v>
@@ -2394,35 +2394,35 @@
       </c>
       <c r="L9" s="24"/>
       <c r="M9" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="N9" s="22"/>
       <c r="P9" s="23" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="Q9" s="23" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="T9" s="23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="V9" s="19" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="W9" s="23" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="X9" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="69.95" customHeight="1">
@@ -2445,7 +2445,7 @@
         <v>110</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H10" s="27" t="s">
         <v>116</v>
@@ -2466,34 +2466,34 @@
         <v>134</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="P10" s="23" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="Q10" s="23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="T10" s="23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="V10" s="19" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="W10" s="23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="X10" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -2548,29 +2548,29 @@
     </row>
     <row r="2" spans="1:7" ht="50.1" customHeight="1">
       <c r="A2" s="19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="50.1" customHeight="1">
       <c r="A3" s="19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="50.1" customHeight="1">
       <c r="A4" s="19" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="2"/>
@@ -2578,10 +2578,10 @@
     </row>
     <row r="5" spans="1:7" ht="50.1" customHeight="1">
       <c r="A5" s="19" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2912,162 +2912,162 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="16" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="16" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="16" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="16" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="16" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="16" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="16" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="16" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="16" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="16" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="16" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="16" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="16" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="16" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="16" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" customHeight="1">
       <c r="A18" s="16" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B18" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" customHeight="1">
       <c r="A19" s="16" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B19" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" customHeight="1">
       <c r="A20" s="16" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -3130,7 +3130,7 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
@@ -3168,17 +3168,17 @@
         <v>101</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E2" s="43"/>
       <c r="F2" s="44" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="I2" s="44"/>
     </row>
@@ -3187,17 +3187,17 @@
         <v>102</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D3" s="44" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E3" s="43"/>
       <c r="F3" s="45" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I3" s="44"/>
     </row>
@@ -3206,17 +3206,17 @@
         <v>103</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C4" s="45" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D4" s="44" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E4" s="43"/>
       <c r="F4" s="45" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="I4" s="45"/>
     </row>
@@ -3225,17 +3225,17 @@
         <v>104</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D5" s="44" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E5" s="43"/>
       <c r="F5" s="45" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="I5" s="44"/>
     </row>
@@ -3304,62 +3304,62 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D2" s="9"/>
       <c r="I2" s="33" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D3" s="5"/>
       <c r="I3" s="33" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D4" s="5"/>
       <c r="I4" s="33" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D5" s="5"/>
       <c r="I5" s="33" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -3438,47 +3438,47 @@
         <v>66</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3526,16 +3526,16 @@
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="26.25" customHeight="1">
       <c r="A2" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>172</v>
-      </c>
       <c r="C2" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -3546,45 +3546,45 @@
         <v>129</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E3" s="12"/>
       <c r="G3" s="31"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>176</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E4" s="5"/>
       <c r="G4" s="31"/>
     </row>
     <row r="5" spans="1:7" ht="60">
       <c r="A5" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E5" s="5"/>
       <c r="G5" s="30"/>
@@ -3594,13 +3594,13 @@
         <v>128</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E6" s="5"/>
       <c r="G6" s="24"/>
@@ -4050,233 +4050,233 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="16" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30">
       <c r="A5" s="16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="16" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="16" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="16" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="16" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="16" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="16" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="16" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="16" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="16" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="16" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="16" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B19" s="38" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1">
       <c r="A20" s="16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B20" s="38" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1">
       <c r="A21" s="16" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B21" s="38" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1">
       <c r="A22" s="16" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1">
       <c r="A23" s="16" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1">
       <c r="A24" s="16" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1">
       <c r="A25" s="16" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B25" s="38" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H25" s="36"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1">
       <c r="A26" s="16" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B26" s="38" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="H26" s="36"/>
     </row>
@@ -4363,54 +4363,54 @@
     </row>
     <row r="2" spans="1:3" ht="39.950000000000003" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="39.950000000000003" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="39.950000000000003" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" ht="39.950000000000003" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" ht="39.950000000000003" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" ht="39.950000000000003" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C7" s="5"/>
     </row>
@@ -4499,20 +4499,20 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -4650,34 +4650,34 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
       <c r="D2" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="3"/>
       <c r="D3" s="24" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="3"/>
       <c r="D4" s="23" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E4" s="3"/>
     </row>

</xml_diff>

<commit_message>
Has Legal Resource is working
</commit_message>
<xml_diff>
--- a/source-data/dataTrento/dataTrento.xlsx
+++ b/source-data/dataTrento/dataTrento.xlsx
@@ -1758,9 +1758,9 @@
   </sheetPr>
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N3" sqref="N3:N10"/>
+      <selection pane="bottomLeft" activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15"/>
@@ -2472,7 +2472,7 @@
         <v>257</v>
       </c>
       <c r="Q10" s="23" t="s">
-        <v>146</v>
+        <v>296</v>
       </c>
       <c r="R10" s="5" t="s">
         <v>187</v>
@@ -2889,7 +2889,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Channel, Cost and Concept are working!
</commit_message>
<xml_diff>
--- a/source-data/dataTrento/dataTrento.xlsx
+++ b/source-data/dataTrento/dataTrento.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6765"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6765" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Public Service" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="339">
   <si>
     <t>Name</t>
   </si>
@@ -735,9 +735,6 @@
   </si>
   <si>
     <t>P6M</t>
-  </si>
-  <si>
-    <t>Label</t>
   </si>
   <si>
     <t>89273F0114CC60DF4F1E4C08C754CA98</t>
@@ -1758,7 +1755,7 @@
   </sheetPr>
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q11" sqref="Q11"/>
     </sheetView>
@@ -1913,10 +1910,10 @@
       </c>
       <c r="N2" s="24"/>
       <c r="P2" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Q2" s="23" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>187</v>
@@ -1928,16 +1925,16 @@
         <v>201</v>
       </c>
       <c r="V2" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="W2" s="23" t="s">
         <v>205</v>
       </c>
       <c r="X2" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:26" s="2" customFormat="1" ht="69.95" customHeight="1">
@@ -1982,10 +1979,10 @@
         <v>182</v>
       </c>
       <c r="P3" s="31" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Q3" s="23" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>188</v>
@@ -1997,16 +1994,16 @@
         <v>202</v>
       </c>
       <c r="V3" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="W3" s="31" t="s">
         <v>206</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="69.95" customHeight="1">
@@ -2050,10 +2047,10 @@
       <c r="N4" s="22"/>
       <c r="O4"/>
       <c r="P4" s="31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="Q4" s="31" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="R4" s="25"/>
       <c r="T4" s="23" t="s">
@@ -2063,14 +2060,14 @@
         <v>203</v>
       </c>
       <c r="V4" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="W4" s="25"/>
       <c r="X4" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="69.95" customHeight="1">
@@ -2118,10 +2115,10 @@
       </c>
       <c r="O5"/>
       <c r="P5" s="31" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Q5" s="23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="R5" s="5" t="s">
         <v>187</v>
@@ -2133,16 +2130,16 @@
         <v>201</v>
       </c>
       <c r="V5" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="W5" s="23" t="s">
         <v>207</v>
       </c>
       <c r="X5" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="69.95" customHeight="1">
@@ -2183,16 +2180,16 @@
         <v>133</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="N6" s="5" t="s">
         <v>184</v>
       </c>
       <c r="P6" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q6" s="23" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="R6" s="5" t="s">
         <v>187</v>
@@ -2204,16 +2201,16 @@
         <v>201</v>
       </c>
       <c r="V6" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="W6" s="23" t="s">
         <v>208</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="69.95" customHeight="1">
@@ -2260,10 +2257,10 @@
         <v>185</v>
       </c>
       <c r="P7" s="31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Q7" s="23" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R7" s="5" t="s">
         <v>187</v>
@@ -2275,16 +2272,16 @@
         <v>201</v>
       </c>
       <c r="V7" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="W7" s="23" t="s">
         <v>207</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="69.95" customHeight="1">
@@ -2325,16 +2322,16 @@
         <v>133</v>
       </c>
       <c r="M8" s="24" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="N8" s="5" t="s">
         <v>186</v>
       </c>
       <c r="P8" s="31" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q8" s="23" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="R8" s="5" t="s">
         <v>187</v>
@@ -2346,16 +2343,16 @@
         <v>201</v>
       </c>
       <c r="V8" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="W8" s="23" t="s">
         <v>209</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="69.95" customHeight="1">
@@ -2398,10 +2395,10 @@
       </c>
       <c r="N9" s="22"/>
       <c r="P9" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Q9" s="23" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="R9" s="5" t="s">
         <v>187</v>
@@ -2413,16 +2410,16 @@
         <v>204</v>
       </c>
       <c r="V9" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W9" s="23" t="s">
         <v>210</v>
       </c>
       <c r="X9" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="69.95" customHeight="1">
@@ -2469,10 +2466,10 @@
         <v>187</v>
       </c>
       <c r="P10" s="23" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Q10" s="23" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="R10" s="5" t="s">
         <v>187</v>
@@ -2484,16 +2481,16 @@
         <v>204</v>
       </c>
       <c r="V10" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W10" s="23" t="s">
         <v>208</v>
       </c>
       <c r="X10" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2548,7 +2545,7 @@
     </row>
     <row r="2" spans="1:7" ht="50.1" customHeight="1">
       <c r="A2" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>150</v>
@@ -2558,7 +2555,7 @@
     </row>
     <row r="3" spans="1:7" ht="50.1" customHeight="1">
       <c r="A3" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>151</v>
@@ -2567,7 +2564,7 @@
     </row>
     <row r="4" spans="1:7" ht="50.1" customHeight="1">
       <c r="A4" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>152</v>
@@ -2578,7 +2575,7 @@
     </row>
     <row r="5" spans="1:7" ht="50.1" customHeight="1">
       <c r="A5" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>153</v>
@@ -2912,159 +2909,159 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="16" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="16" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" customHeight="1">
       <c r="A18" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" customHeight="1">
       <c r="A19" s="16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" customHeight="1">
       <c r="A20" s="16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>146</v>
@@ -3168,17 +3165,17 @@
         <v>101</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D2" s="44" t="s">
         <v>149</v>
       </c>
       <c r="E2" s="43"/>
       <c r="F2" s="44" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I2" s="44"/>
     </row>
@@ -3187,17 +3184,17 @@
         <v>102</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D3" s="44" t="s">
         <v>149</v>
       </c>
       <c r="E3" s="43"/>
       <c r="F3" s="45" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I3" s="44"/>
     </row>
@@ -3206,17 +3203,17 @@
         <v>103</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C4" s="45" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D4" s="44" t="s">
         <v>149</v>
       </c>
       <c r="E4" s="43"/>
       <c r="F4" s="45" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I4" s="45"/>
     </row>
@@ -3225,17 +3222,17 @@
         <v>104</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D5" s="44" t="s">
         <v>149</v>
       </c>
       <c r="E5" s="43"/>
       <c r="F5" s="45" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I5" s="44"/>
     </row>
@@ -3425,7 +3422,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3438,12 +3437,12 @@
         <v>66</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>211</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>157</v>
@@ -3451,7 +3450,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>158</v>
@@ -3459,7 +3458,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B4" s="23" t="s">
         <v>159</v>
@@ -3467,7 +3466,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>160</v>
@@ -3475,7 +3474,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B6" s="24" t="s">
         <v>161</v>
@@ -4050,233 +4049,233 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30">
       <c r="A5" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B19" s="38" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1">
       <c r="A20" s="16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B20" s="38" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1">
       <c r="A21" s="16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B21" s="38" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1">
       <c r="A22" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1">
       <c r="A23" s="16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1">
       <c r="A24" s="16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1">
       <c r="A25" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B25" s="38" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H25" s="36"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1">
       <c r="A26" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B26" s="38" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H26" s="36"/>
     </row>
@@ -4613,11 +4612,11 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -4650,7 +4649,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
@@ -4661,7 +4660,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="3"/>
@@ -4672,7 +4671,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="3"/>
@@ -4680,6 +4679,36 @@
         <v>156</v>
       </c>
       <c r="E4" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="31" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="45" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="44" t="s">
+        <v>156</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4689,14 +4718,75 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PwC_JobCode xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">F049</PwC_JobCode>
+    <PwC_JobSearch xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">F049 - ABCIII SC270</PwC_JobSearch>
+    <PwC_FiscalYear xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">FY17</PwC_FiscalYear>
+    <PwC_Language xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">EN</PwC_Language>
+    <PwC_ExpirationDate xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">2023-07-10T22:00:00+00:00</PwC_ExpirationDate>
+    <PwC_ClientCode xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">86155139</PwC_ClientCode>
+    <RelatedItems xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PwC_ClientSearch xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">86155139 - DG INFORMATICS (DIGIT)</PwC_ClientSearch>
+    <_dlc_DocId xmlns="73fde05d-ef26-44d0-b13b-b564e323f6a1">SK445ZKHUCMR-447-133</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="73fde05d-ef26-44d0-b13b-b564e323f6a1">
+      <Url>https://be-docbox.be.ema.pwcinternal.com/sites/10014628/86155139F049/_layouts/15/DocIdRedir.aspx?ID=SK445ZKHUCMR-447-133</Url>
+      <Description>SK445ZKHUCMR-447-133</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="PwC Job Document" ma:contentTypeID="0x0101008E49C3D400044AB3A2F1DD14073E74F6001D06D12572244BE3A11AAEE3ED60F576000AAB1FD6C2134AF1A3EA6F52344189D8003DA7CBE2F9F6014D91228B237B0D6438" ma:contentTypeVersion="2" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="3d6a3c6679c05d12a3160ad00a1d5007">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="73fde05d-ef26-44d0-b13b-b564e323f6a1" xmlns:ns3="885fffe5-095f-4e72-b33a-2965af2fc427" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e9ac53f853e0ef9b3d9397434b7eb735" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4907,85 +4997,42 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PwC_JobCode xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">F049</PwC_JobCode>
-    <PwC_JobSearch xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">F049 - ABCIII SC270</PwC_JobSearch>
-    <PwC_FiscalYear xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">FY17</PwC_FiscalYear>
-    <PwC_Language xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">EN</PwC_Language>
-    <PwC_ExpirationDate xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">2023-07-10T22:00:00+00:00</PwC_ExpirationDate>
-    <PwC_ClientCode xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">86155139</PwC_ClientCode>
-    <RelatedItems xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PwC_ClientSearch xmlns="885fffe5-095f-4e72-b33a-2965af2fc427">86155139 - DG INFORMATICS (DIGIT)</PwC_ClientSearch>
-    <_dlc_DocId xmlns="73fde05d-ef26-44d0-b13b-b564e323f6a1">SK445ZKHUCMR-447-133</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="73fde05d-ef26-44d0-b13b-b564e323f6a1">
-      <Url>https://be-docbox.be.ema.pwcinternal.com/sites/10014628/86155139F049/_layouts/15/DocIdRedir.aspx?ID=SK445ZKHUCMR-447-133</Url>
-      <Description>SK445ZKHUCMR-447-133</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08E82FCB-F73C-4EEA-86B9-8873465BC0AE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704B0184-4F17-45F2-9AC0-8A30DB782E6F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B2323CD-3102-47C1-AE6C-40C0EBF3BFA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="73fde05d-ef26-44d0-b13b-b564e323f6a1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="885fffe5-095f-4e72-b33a-2965af2fc427"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10E94497-4933-4E21-9510-AD09FE48006D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5005,28 +5052,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B2323CD-3102-47C1-AE6C-40C0EBF3BFA9}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08E82FCB-F73C-4EEA-86B9-8873465BC0AE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="73fde05d-ef26-44d0-b13b-b564e323f6a1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="885fffe5-095f-4e72-b33a-2965af2fc427"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704B0184-4F17-45F2-9AC0-8A30DB782E6F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Improved code a lot
</commit_message>
<xml_diff>
--- a/source-data/dataTrento/dataTrento.xlsx
+++ b/source-data/dataTrento/dataTrento.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" firstSheet="6" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Public Service" sheetId="1" r:id="rId1"/>
     <sheet name="Business Event" sheetId="2" r:id="rId2"/>
     <sheet name="Life Event" sheetId="3" r:id="rId3"/>
-    <sheet name="Public Service Dataset" sheetId="4" r:id="rId4"/>
+    <sheet name="PS Dataset" sheetId="4" r:id="rId4"/>
     <sheet name="Participation" sheetId="5" r:id="rId5"/>
     <sheet name="Criterion Requirement" sheetId="6" r:id="rId6"/>
     <sheet name="Evidence" sheetId="7" r:id="rId7"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1820" uniqueCount="1115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1817" uniqueCount="1113">
   <si>
     <t>PSURI</t>
   </si>
@@ -2634,9 +2634,6 @@
     <t>if Accessed Through</t>
   </si>
   <si>
-    <t>EUR-Euro</t>
-  </si>
-  <si>
     <t>Marca da bollo da 16 euro, se non esenti</t>
   </si>
   <si>
@@ -3735,9 +3732,6 @@
   </si>
   <si>
     <t>OutputURI</t>
-  </si>
-  <si>
-    <t>Identifier</t>
   </si>
   <si>
     <t>Contributi</t>
@@ -8510,22 +8504,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>812</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>813</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>814</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>815</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>816</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>817</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -9537,7 +9531,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -9549,7 +9543,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -10560,7 +10554,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="32" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -10571,90 +10565,90 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="34" t="s">
+        <v>820</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>821</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="35" t="s">
+        <v>822</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>823</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="34" t="s">
+        <v>824</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>825</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="35" t="s">
+        <v>826</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>827</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="34" t="s">
+        <v>828</v>
+      </c>
+      <c r="B6" s="36" t="s">
         <v>829</v>
-      </c>
-      <c r="B6" s="36" t="s">
-        <v>830</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="35" t="s">
+        <v>830</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>831</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>832</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="35" t="s">
+        <v>832</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>833</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="35" t="s">
+        <v>834</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>835</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>836</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="35" t="s">
+        <v>836</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>837</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>838</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="34" t="s">
+        <v>838</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>839</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="35" t="s">
+        <v>840</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>841</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>842</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -10662,95 +10656,95 @@
         <v>140</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="35" t="s">
+        <v>843</v>
+      </c>
+      <c r="B14" s="36" t="s">
         <v>844</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>845</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="35" t="s">
+        <v>845</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>846</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>847</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="35" t="s">
+        <v>847</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>848</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>849</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="35" t="s">
+        <v>849</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>850</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="35" t="s">
+        <v>851</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>852</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>853</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="35" t="s">
+        <v>853</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>854</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>855</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="34" t="s">
+        <v>855</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>856</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="35" t="s">
+        <v>857</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>858</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>859</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="34" t="s">
+        <v>859</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>860</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="35" t="s">
+        <v>861</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>862</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="34" t="s">
+        <v>863</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>864</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>865</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -10758,119 +10752,119 @@
         <v>55</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="34" t="s">
+        <v>866</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>867</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>868</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="35" t="s">
+        <v>868</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>869</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>870</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="34" t="s">
+        <v>870</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>871</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>872</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="34" t="s">
+        <v>872</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>873</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>874</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="34" t="s">
+        <v>874</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>875</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="34" t="s">
+        <v>876</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>877</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>878</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="34" t="s">
+        <v>878</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>879</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>880</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="35" t="s">
+        <v>880</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>881</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>882</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="35" t="s">
+        <v>882</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>883</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>884</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="35" t="s">
+        <v>884</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>885</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>886</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="35" t="s">
+        <v>886</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>887</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>888</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="35" t="s">
+        <v>888</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>889</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>890</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="34" t="s">
+        <v>890</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>891</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>892</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="34" t="s">
+        <v>892</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>893</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>894</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
@@ -10878,47 +10872,47 @@
         <v>281</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="34" t="s">
+        <v>895</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>896</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>897</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="35" t="s">
+        <v>897</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>898</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>899</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="35" t="s">
+        <v>899</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>900</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>901</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="35" t="s">
+        <v>901</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>902</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>903</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="35" t="s">
+        <v>903</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>904</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>905</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -10926,247 +10920,247 @@
         <v>271</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="35" t="s">
+        <v>906</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>907</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>908</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="34" t="s">
+        <v>908</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>909</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>910</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="34" t="s">
+        <v>910</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>911</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="34" t="s">
+        <v>912</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>913</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>914</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="35" t="s">
+        <v>914</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>915</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>916</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="34" t="s">
+        <v>916</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>917</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>918</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="35" t="s">
+        <v>918</v>
+      </c>
+      <c r="B53" s="36" t="s">
         <v>919</v>
-      </c>
-      <c r="B53" s="36" t="s">
-        <v>920</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="34" t="s">
+        <v>920</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>921</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>922</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="34" t="s">
+        <v>922</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>923</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>924</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="34" t="s">
+        <v>924</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>925</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>926</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="35" t="s">
+        <v>926</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>927</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>928</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="34" t="s">
+        <v>928</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>929</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>930</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="34" t="s">
+        <v>930</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>931</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>932</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="34" t="s">
+        <v>932</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>933</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>934</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="34" t="s">
+        <v>934</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>935</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>936</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="34" t="s">
+        <v>936</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>937</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>938</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="35" t="s">
+        <v>938</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>939</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>940</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="34" t="s">
+        <v>940</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>941</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>942</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="34" t="s">
+        <v>942</v>
+      </c>
+      <c r="B65" s="5" t="s">
         <v>943</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>944</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="34" t="s">
+        <v>944</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>945</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>946</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="35" t="s">
+        <v>946</v>
+      </c>
+      <c r="B67" s="5" t="s">
         <v>947</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>948</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="35" t="s">
+        <v>948</v>
+      </c>
+      <c r="B68" s="5" t="s">
         <v>949</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>950</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="35" t="s">
+        <v>950</v>
+      </c>
+      <c r="B69" s="5" t="s">
         <v>951</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>952</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="35" t="s">
+        <v>952</v>
+      </c>
+      <c r="B70" s="5" t="s">
         <v>953</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>954</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="35" t="s">
+        <v>954</v>
+      </c>
+      <c r="B71" s="5" t="s">
         <v>955</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>956</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="34" t="s">
+        <v>956</v>
+      </c>
+      <c r="B72" s="5" t="s">
         <v>957</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>958</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="34" t="s">
+        <v>958</v>
+      </c>
+      <c r="B73" s="5" t="s">
         <v>959</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>960</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="34" t="s">
+        <v>960</v>
+      </c>
+      <c r="B74" s="5" t="s">
         <v>961</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>962</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="35" t="s">
+        <v>962</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>964</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="35" t="s">
+        <v>964</v>
+      </c>
+      <c r="B76" s="5" t="s">
         <v>965</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>966</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -11174,7 +11168,7 @@
         <v>455</v>
       </c>
       <c r="B77" s="36" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -11182,23 +11176,23 @@
         <v>244</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="35" t="s">
+        <v>968</v>
+      </c>
+      <c r="B79" s="5" t="s">
         <v>969</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>970</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="34" t="s">
+        <v>970</v>
+      </c>
+      <c r="B80" s="5" t="s">
         <v>971</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>972</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -11206,23 +11200,23 @@
         <v>38</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="35" t="s">
+        <v>973</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>974</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>975</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="35" t="s">
+        <v>975</v>
+      </c>
+      <c r="B83" s="36" t="s">
         <v>976</v>
-      </c>
-      <c r="B83" s="36" t="s">
-        <v>977</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -11230,63 +11224,63 @@
         <v>68</v>
       </c>
       <c r="B84" s="36" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="35" t="s">
+        <v>978</v>
+      </c>
+      <c r="B85" s="5" t="s">
         <v>979</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>980</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="34" t="s">
+        <v>980</v>
+      </c>
+      <c r="B86" s="36" t="s">
         <v>981</v>
-      </c>
-      <c r="B86" s="36" t="s">
-        <v>982</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="B87" s="5" t="s">
         <v>983</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>984</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="34" t="s">
+        <v>984</v>
+      </c>
+      <c r="B88" s="5" t="s">
         <v>985</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>986</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="34" t="s">
+        <v>986</v>
+      </c>
+      <c r="B89" s="3" t="s">
         <v>987</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>988</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="34" t="s">
+        <v>988</v>
+      </c>
+      <c r="B90" s="5" t="s">
         <v>989</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>990</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="34" t="s">
+        <v>990</v>
+      </c>
+      <c r="B91" s="5" t="s">
         <v>991</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>992</v>
       </c>
     </row>
   </sheetData>
@@ -11317,16 +11311,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>994</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>995</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -12341,22 +12335,22 @@
   <sheetData>
     <row r="1" spans="1:26" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>994</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>995</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="43.5" x14ac:dyDescent="0.35">
@@ -12364,17 +12358,17 @@
         <v>29</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="G2" s="36"/>
       <c r="H2" s="36"/>
@@ -12402,17 +12396,17 @@
         <v>47</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="G3" s="36"/>
       <c r="H3" s="36"/>
@@ -12440,17 +12434,17 @@
         <v>276</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -12478,17 +12472,17 @@
         <v>289</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="G5" s="36"/>
       <c r="H5" s="36"/>
@@ -12516,17 +12510,17 @@
         <v>360</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="G6" s="36"/>
       <c r="H6" s="36"/>
@@ -12554,17 +12548,17 @@
         <v>133</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>39</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="G7" s="36"/>
       <c r="H7" s="36"/>
@@ -12592,17 +12586,17 @@
         <v>160</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>39</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="G8" s="36"/>
       <c r="H8" s="36"/>
@@ -12630,17 +12624,17 @@
         <v>240</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>39</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="G9" s="36"/>
       <c r="H9" s="36"/>
@@ -12668,17 +12662,17 @@
         <v>252</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>39</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="G10" s="36"/>
       <c r="H10" s="36"/>
@@ -12706,17 +12700,17 @@
         <v>173</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>39</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="G11" s="36"/>
       <c r="H11" s="36"/>
@@ -12744,17 +12738,17 @@
         <v>337</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>39</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="G12" s="36"/>
       <c r="H12" s="36"/>
@@ -12782,17 +12776,17 @@
         <v>348</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>39</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="G13" s="36"/>
       <c r="H13" s="36"/>
@@ -12820,17 +12814,17 @@
         <v>110</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="G14" s="36"/>
       <c r="H14" s="36"/>
@@ -12858,17 +12852,17 @@
         <v>327</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="24" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -13850,43 +13844,43 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1021</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1022</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1023</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1024</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1025</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>1026</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="C2" s="37" t="s">
         <v>1027</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>1028</v>
       </c>
       <c r="D2" s="24"/>
       <c r="E2" s="37" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="24" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>1030</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>1031</v>
       </c>
       <c r="C3" s="37"/>
       <c r="D3" s="24"/>
@@ -13895,10 +13889,10 @@
     </row>
     <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="24" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B4" s="24" t="s">
         <v>1032</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>1033</v>
       </c>
       <c r="C4" s="37"/>
       <c r="D4" s="24"/>
@@ -13907,10 +13901,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>1034</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>1035</v>
       </c>
       <c r="C5" s="38"/>
       <c r="D5" s="24"/>
@@ -13922,39 +13916,39 @@
         <v>177</v>
       </c>
       <c r="B6" s="24" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C6" s="37" t="s">
         <v>1036</v>
-      </c>
-      <c r="C6" s="37" t="s">
-        <v>1037</v>
       </c>
       <c r="D6" s="24"/>
       <c r="E6" s="37" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="27" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B7" s="24" t="s">
         <v>1039</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="C7" s="37" t="s">
         <v>1040</v>
-      </c>
-      <c r="C7" s="37" t="s">
-        <v>1041</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="37" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="27" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>1043</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>1044</v>
       </c>
       <c r="C8" s="37"/>
       <c r="D8" s="24"/>
@@ -13963,26 +13957,26 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="27" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>1045</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="C9" s="37" t="s">
         <v>1046</v>
-      </c>
-      <c r="C9" s="37" t="s">
-        <v>1047</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="37" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="27" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B10" s="27" t="s">
         <v>1049</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>1050</v>
       </c>
       <c r="C10" s="37"/>
       <c r="D10" s="24"/>
@@ -13994,26 +13988,26 @@
         <v>165</v>
       </c>
       <c r="B11" s="24" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C11" s="37" t="s">
         <v>1051</v>
-      </c>
-      <c r="C11" s="37" t="s">
-        <v>1052</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="37" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="27" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B12" s="27" t="s">
         <v>1054</v>
       </c>
-      <c r="B12" s="27" t="s">
-        <v>1055</v>
-      </c>
       <c r="C12" s="27" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="D12" s="39"/>
       <c r="E12" s="39"/>
@@ -14021,10 +14015,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="27" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B13" s="27" t="s">
         <v>1056</v>
-      </c>
-      <c r="B13" s="27" t="s">
-        <v>1057</v>
       </c>
       <c r="C13" s="37"/>
       <c r="D13" s="39"/>
@@ -14036,10 +14030,10 @@
         <v>217</v>
       </c>
       <c r="B14" s="27" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C14" s="37" t="s">
         <v>1058</v>
-      </c>
-      <c r="C14" s="37" t="s">
-        <v>1059</v>
       </c>
       <c r="D14" s="39"/>
       <c r="E14" s="39"/>
@@ -14047,13 +14041,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B15" s="27" t="s">
         <v>1060</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="C15" s="37" t="s">
         <v>1061</v>
-      </c>
-      <c r="C15" s="37" t="s">
-        <v>1062</v>
       </c>
       <c r="D15" s="39"/>
       <c r="E15" s="39"/>
@@ -14061,10 +14055,10 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B16" s="27" t="s">
         <v>1063</v>
-      </c>
-      <c r="B16" s="27" t="s">
-        <v>1064</v>
       </c>
       <c r="C16" s="39"/>
       <c r="D16" s="39"/>
@@ -14073,25 +14067,25 @@
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="24" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B17" s="24" t="s">
         <v>1065</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="C17" s="40" t="s">
         <v>1066</v>
-      </c>
-      <c r="C17" s="40" t="s">
-        <v>1067</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="40" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="24" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B18" s="25" t="s">
         <v>1069</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>1070</v>
       </c>
       <c r="C18" s="40"/>
       <c r="D18" s="25"/>
@@ -14099,25 +14093,25 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="24" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B19" s="24" t="s">
         <v>1071</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="C19" s="40" t="s">
         <v>1072</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>1073</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19" s="40" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="24" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B20" s="25" t="s">
         <v>1075</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>1076</v>
       </c>
       <c r="C20" s="40"/>
       <c r="D20" s="25"/>
@@ -14125,25 +14119,25 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="24" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B21" s="24" t="s">
         <v>1077</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="C21" s="40" t="s">
         <v>1078</v>
-      </c>
-      <c r="C21" s="40" t="s">
-        <v>1079</v>
       </c>
       <c r="D21" s="25"/>
       <c r="E21" s="40" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="24" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B22" s="25" t="s">
         <v>1081</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>1082</v>
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="25"/>
@@ -14151,25 +14145,25 @@
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="25" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B23" s="25" t="s">
         <v>1083</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="C23" s="40" t="s">
         <v>1084</v>
-      </c>
-      <c r="C23" s="40" t="s">
-        <v>1085</v>
       </c>
       <c r="D23" s="25"/>
       <c r="E23" s="40" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="25" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B24" s="25" t="s">
         <v>1087</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>1088</v>
       </c>
       <c r="C24" s="25"/>
       <c r="D24" s="25"/>
@@ -14177,25 +14171,25 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="25" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B25" s="25" t="s">
         <v>1089</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="C25" s="25" t="s">
         <v>1090</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>1091</v>
       </c>
       <c r="D25" s="25"/>
       <c r="E25" s="40" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="25" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B26" s="25" t="s">
         <v>1093</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>1094</v>
       </c>
       <c r="C26" s="25"/>
       <c r="D26" s="25"/>
@@ -14203,25 +14197,25 @@
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B27" s="25" t="s">
         <v>1095</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="C27" s="25" t="s">
         <v>1096</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>1097</v>
       </c>
       <c r="D27" s="25"/>
       <c r="E27" s="40" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B28" s="25" t="s">
         <v>1099</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>1100</v>
       </c>
       <c r="C28" s="41"/>
       <c r="D28" s="41"/>
@@ -14237,7 +14231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -15256,103 +15250,94 @@
   <sheetPr>
     <tabColor rgb="FF5B9BD5"/>
   </sheetPr>
-  <dimension ref="A1:E1000"/>
+  <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.6328125"/>
-    <col min="2" max="2" width="15.26953125"/>
-    <col min="3" max="3" width="37.54296875"/>
-    <col min="4" max="4" width="11.36328125"/>
-    <col min="5" max="26" width="14.81640625"/>
-    <col min="27" max="1025" width="14.1796875"/>
+    <col min="2" max="2" width="37.54296875"/>
+    <col min="3" max="3" width="11.36328125"/>
+    <col min="4" max="25" width="14.81640625"/>
+    <col min="26" max="1024" width="14.1796875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1102</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="44" t="s">
-        <v>1103</v>
-      </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44" t="s">
-        <v>1104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B2" s="44" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="35" t="s">
-        <v>1105</v>
-      </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="35" t="s">
-        <v>1106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B3" s="35" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C3" s="41"/>
+      <c r="D3" s="35" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="35" t="s">
         <v>397</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="35" t="s">
-        <v>1107</v>
-      </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="35" t="s">
-        <v>1108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B4" s="35" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C4" s="41"/>
+      <c r="D4" s="35" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="35" t="s">
         <v>424</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="35" t="s">
-        <v>1109</v>
-      </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="35" t="s">
-        <v>1110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B5" s="35" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C5" s="41"/>
+      <c r="D5" s="35" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="35" t="s">
-        <v>1111</v>
-      </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="35" t="s">
-        <v>1112</v>
+      <c r="B6" s="35" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C6" s="41"/>
+      <c r="D6" s="35" t="s">
+        <v>1110</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -16355,7 +16340,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -20041,9 +20026,9 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27182,8 +27167,8 @@
   <dimension ref="A1:F1031"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27222,14 +27207,10 @@
       <c r="A2" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="28">
-        <v>16</v>
-      </c>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29" t="s">
         <v>758</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>759</v>
       </c>
       <c r="E2" s="30"/>
     </row>
@@ -27237,47 +27218,43 @@
       <c r="A3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="31">
-        <v>0</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>758</v>
-      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="25"/>
       <c r="D3" s="25" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E3" s="30"/>
     </row>
     <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
       <c r="D4" s="25" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E4" s="30"/>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B5" s="25"/>
       <c r="C5" s="25"/>
       <c r="D5" s="25" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E5" s="30"/>
     </row>
     <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E6" s="30"/>
     </row>
@@ -27288,7 +27265,7 @@
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
       <c r="D7" s="25" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E7" s="30"/>
     </row>
@@ -27299,7 +27276,7 @@
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
       <c r="D8" s="4" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="E8" s="30"/>
     </row>
@@ -27310,7 +27287,7 @@
       <c r="B9" s="25"/>
       <c r="C9" s="25"/>
       <c r="D9" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="E9" s="30"/>
     </row>
@@ -27321,7 +27298,7 @@
       <c r="B10" s="25"/>
       <c r="C10" s="25"/>
       <c r="D10" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E10" s="30"/>
     </row>
@@ -27332,7 +27309,7 @@
       <c r="B11" s="25"/>
       <c r="C11" s="25"/>
       <c r="D11" s="5" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E11" s="30"/>
     </row>
@@ -27343,7 +27320,7 @@
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
       <c r="D12" s="5" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E12" s="30"/>
     </row>
@@ -27354,7 +27331,7 @@
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
       <c r="D13" s="5" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E13" s="30"/>
     </row>
@@ -27365,7 +27342,7 @@
       <c r="B14" s="25"/>
       <c r="C14" s="25"/>
       <c r="D14" s="5" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E14" s="30"/>
     </row>
@@ -27376,7 +27353,7 @@
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
       <c r="D15" s="5" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E15" s="30"/>
     </row>
@@ -27387,7 +27364,7 @@
       <c r="B16" s="25"/>
       <c r="C16" s="25"/>
       <c r="D16" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E16" s="30"/>
     </row>
@@ -27398,7 +27375,7 @@
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
       <c r="D17" s="5" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E17" s="30"/>
     </row>
@@ -27409,7 +27386,7 @@
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
       <c r="D18" s="5" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="E18" s="30"/>
     </row>
@@ -28423,13 +28400,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="32" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B1" s="33" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D1" s="33" t="s">
         <v>7</v>
@@ -28438,10 +28415,10 @@
         <v>15</v>
       </c>
       <c r="F1" s="33" t="s">
+        <v>779</v>
+      </c>
+      <c r="G1" s="33" t="s">
         <v>780</v>
-      </c>
-      <c r="G1" s="33" t="s">
-        <v>781</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="56" x14ac:dyDescent="0.35">
@@ -28449,7 +28426,7 @@
         <v>41</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C2" s="4"/>
     </row>
@@ -28458,7 +28435,7 @@
         <v>58</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -28467,7 +28444,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="30"/>
@@ -28477,7 +28454,7 @@
         <v>80</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C5" s="5"/>
       <c r="E5" s="4"/>
@@ -28487,7 +28464,7 @@
         <v>92</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C6" s="5"/>
     </row>
@@ -28496,7 +28473,7 @@
         <v>104</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C7" s="4"/>
     </row>
@@ -28505,7 +28482,7 @@
         <v>116</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C8" s="4"/>
     </row>
@@ -28514,7 +28491,7 @@
         <v>127</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C9" s="5"/>
     </row>
@@ -28523,7 +28500,7 @@
         <v>142</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C10" s="3"/>
     </row>
@@ -28532,7 +28509,7 @@
         <v>155</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C11" s="5"/>
     </row>
@@ -28541,7 +28518,7 @@
         <v>166</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C12" s="3"/>
     </row>
@@ -28550,7 +28527,7 @@
         <v>178</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C13" s="3"/>
     </row>
@@ -28559,7 +28536,7 @@
         <v>224</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C14" s="3"/>
     </row>
@@ -28568,7 +28545,7 @@
         <v>246</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C15" s="3"/>
     </row>
@@ -28577,7 +28554,7 @@
         <v>262</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C16" s="3"/>
     </row>
@@ -28586,7 +28563,7 @@
         <v>284</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C17" s="3"/>
     </row>
@@ -28595,7 +28572,7 @@
         <v>296</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C18" s="3"/>
     </row>
@@ -28604,7 +28581,7 @@
         <v>305</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C19" s="3"/>
     </row>
@@ -28613,7 +28590,7 @@
         <v>315</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C20" s="3"/>
     </row>
@@ -28622,7 +28599,7 @@
         <v>322</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C21" s="3"/>
     </row>
@@ -28631,7 +28608,7 @@
         <v>332</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C22" s="3"/>
     </row>
@@ -28640,7 +28617,7 @@
         <v>355</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C23" s="4"/>
     </row>
@@ -28649,7 +28626,7 @@
         <v>367</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="C24" s="3"/>
     </row>
@@ -28658,7 +28635,7 @@
         <v>377</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C25" s="3"/>
     </row>
@@ -28667,7 +28644,7 @@
         <v>435</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="C26" s="3"/>
     </row>
@@ -28676,7 +28653,7 @@
         <v>466</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C27" s="3"/>
     </row>
@@ -28685,7 +28662,7 @@
         <v>477</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C28" s="4"/>
     </row>
@@ -28694,7 +28671,7 @@
         <v>494</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C29" s="3"/>
     </row>
@@ -28703,7 +28680,7 @@
         <v>506</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C30" s="3"/>
     </row>
@@ -28712,7 +28689,7 @@
         <v>517</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C31" s="3"/>
     </row>

</xml_diff>